<commit_message>
Add HTML to Esemenyek.xlsx
</commit_message>
<xml_diff>
--- a/Docs/Specs/Esemenyek.xlsx
+++ b/Docs/Specs/Esemenyek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bzfel\source\repos\Kantoratus\Docs\Specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7AFB05-7519-4573-9B14-24EC9267A7D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF92038B-B4CF-4996-8861-8AE96060BD69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1849B515-BAB5-47C1-853D-034EF5E07261}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Év</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Kelenföldi evangélikus templom</t>
   </si>
   <si>
-    <t>A vesperák az egyházi év vasárnapjainak megfelelően változó anyagát a Gyülekezeti liturgikus könyv 2007-es megjelenéséig az ünnepkörönként változó „küllap” és az adott vasárnap jellegét tükröző „bellap” kombinálásával adhattuk a gyülekezeti tagok kezébe. A kezdeti időszakban szöveges magyarázat is segítette a tájékozódást.</t>
-  </si>
-  <si>
     <t>Az első vespera</t>
   </si>
   <si>
@@ -76,6 +73,13 @@
   </si>
   <si>
     <t>Közös vesperás a Soli Deo Gloria kamarakórussal (vez. Bódiss Tamás)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A vesperák az egyházi év vasárnapjainak megfelelően változó anyagát a Gyülekezeti liturgikus könyv 2007-es megjelenéséig az ünnepkörönként változó „küllap” és az adott vasárnap jellegét tükröző „bellap” kombinálásával adhattuk a gyülekezeti tagok kezébe. A kezdeti időszakban szöveges magyarázat is segítette a tájékozódást.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Első bekezdés&lt;/p&gt;
+&lt;p&gt;Második bekezdés&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -118,9 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -471,7 +478,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,13 +531,13 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1996</v>
       </c>
@@ -538,13 +545,16 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>